<commit_message>
ek nayi file bnaya
</commit_message>
<xml_diff>
--- a/BOQ-CHILLED WATER.xlsx
+++ b/BOQ-CHILLED WATER.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aamir Suhail\Desktop\SHAHEEM ANJUM\SHAHEEM ANJUM 1\ARCH SAUD RESIDENTIAL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3765F525-4B2C-4035-8ACF-872C89A99AAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7635213-6885-4118-8DF9-5D274279E558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D32A7053-38C2-49EF-846F-B708606C48CC}"/>
+    <workbookView xWindow="3552" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{D32A7053-38C2-49EF-846F-B708606C48CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="22">
   <si>
     <t>BILL OF QUANTITY</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>T-JOINT</t>
+  </si>
+  <si>
+    <t>hjgjhghj</t>
   </si>
 </sst>
 </file>
@@ -472,18 +475,85 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -493,79 +563,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -883,10 +886,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="E2:S37"/>
+  <dimension ref="E2:T37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="V16" sqref="V16"/>
+      <selection activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -896,114 +899,114 @@
     <col min="8" max="8" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="5:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E2" s="25" t="s">
+    <row r="2" spans="5:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E2" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
-      <c r="N2" s="25"/>
-      <c r="O2" s="25"/>
-      <c r="P2" s="25"/>
-      <c r="Q2" s="25"/>
-      <c r="R2" s="25"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+      <c r="Q2" s="29"/>
+      <c r="R2" s="29"/>
       <c r="S2" s="1"/>
     </row>
-    <row r="3" spans="5:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="25"/>
-      <c r="N3" s="25"/>
-      <c r="O3" s="25"/>
-      <c r="P3" s="25"/>
-      <c r="Q3" s="25"/>
-      <c r="R3" s="25"/>
+    <row r="3" spans="5:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="29"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="29"/>
+      <c r="Q3" s="29"/>
+      <c r="R3" s="29"/>
       <c r="S3" s="1"/>
     </row>
-    <row r="4" spans="5:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="25"/>
-      <c r="J4" s="25"/>
-      <c r="K4" s="25"/>
-      <c r="L4" s="25"/>
-      <c r="M4" s="25"/>
-      <c r="N4" s="25"/>
-      <c r="O4" s="25"/>
-      <c r="P4" s="25"/>
-      <c r="Q4" s="25"/>
-      <c r="R4" s="25"/>
+    <row r="4" spans="5:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="29"/>
+      <c r="L4" s="29"/>
+      <c r="M4" s="29"/>
+      <c r="N4" s="29"/>
+      <c r="O4" s="29"/>
+      <c r="P4" s="29"/>
+      <c r="Q4" s="29"/>
+      <c r="R4" s="29"/>
       <c r="S4" s="1"/>
     </row>
-    <row r="5" spans="5:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
-      <c r="M5" s="20"/>
-      <c r="N5" s="20"/>
-      <c r="O5" s="20"/>
-      <c r="P5" s="20"/>
-      <c r="Q5" s="20"/>
-      <c r="R5" s="20"/>
-    </row>
-    <row r="6" spans="5:19" ht="18" x14ac:dyDescent="0.3">
-      <c r="E6" s="34" t="s">
+    <row r="5" spans="5:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="30"/>
+      <c r="K5" s="30"/>
+      <c r="L5" s="30"/>
+      <c r="M5" s="30"/>
+      <c r="N5" s="30"/>
+      <c r="O5" s="30"/>
+      <c r="P5" s="30"/>
+      <c r="Q5" s="30"/>
+      <c r="R5" s="30"/>
+    </row>
+    <row r="6" spans="5:20" ht="18" x14ac:dyDescent="0.3">
+      <c r="E6" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="36" t="s">
+      <c r="F6" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="G6" s="36" t="s">
+      <c r="G6" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="H6" s="36" t="s">
+      <c r="H6" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="26" t="s">
+      <c r="I6" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="J6" s="26"/>
-      <c r="K6" s="26" t="s">
+      <c r="J6" s="31"/>
+      <c r="K6" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="L6" s="26"/>
-      <c r="M6" s="26" t="s">
+      <c r="L6" s="31"/>
+      <c r="M6" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="N6" s="26"/>
-      <c r="O6" s="26" t="s">
+      <c r="N6" s="31"/>
+      <c r="O6" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="P6" s="26"/>
-      <c r="Q6" s="30" t="s">
+      <c r="P6" s="31"/>
+      <c r="Q6" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="R6" s="31"/>
-    </row>
-    <row r="7" spans="5:19" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E7" s="35"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
+      <c r="R6" s="19"/>
+    </row>
+    <row r="7" spans="5:20" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E7" s="23"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
       <c r="I7" s="7" t="s">
         <v>4</v>
       </c>
@@ -1016,22 +1019,22 @@
       <c r="L7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="M7" s="27" t="s">
+      <c r="M7" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="N7" s="27"/>
-      <c r="O7" s="27" t="s">
+      <c r="N7" s="32"/>
+      <c r="O7" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="P7" s="27"/>
-      <c r="Q7" s="32"/>
-      <c r="R7" s="33"/>
-    </row>
-    <row r="8" spans="5:19" ht="18" x14ac:dyDescent="0.35">
-      <c r="E8" s="15">
+      <c r="P7" s="32"/>
+      <c r="Q7" s="20"/>
+      <c r="R7" s="21"/>
+    </row>
+    <row r="8" spans="5:20" ht="18" x14ac:dyDescent="0.35">
+      <c r="E8" s="38">
         <v>1</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="34" t="s">
         <v>15</v>
       </c>
       <c r="G8" s="8" t="s">
@@ -1054,24 +1057,24 @@
         <f t="shared" si="0"/>
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="M8" s="28">
+      <c r="M8" s="16">
         <v>2340</v>
       </c>
-      <c r="N8" s="28"/>
-      <c r="O8" s="28">
+      <c r="N8" s="16"/>
+      <c r="O8" s="16">
         <f>M8/1000</f>
         <v>2.34</v>
       </c>
-      <c r="P8" s="28"/>
-      <c r="Q8" s="28">
+      <c r="P8" s="16"/>
+      <c r="Q8" s="16">
         <f>2*O8*(K8+L8)</f>
         <v>0.29952000000000001</v>
       </c>
-      <c r="R8" s="29"/>
-    </row>
-    <row r="9" spans="5:19" ht="18" x14ac:dyDescent="0.35">
-      <c r="E9" s="16"/>
-      <c r="F9" s="13"/>
+      <c r="R8" s="17"/>
+    </row>
+    <row r="9" spans="5:20" ht="18" x14ac:dyDescent="0.35">
+      <c r="E9" s="39"/>
+      <c r="F9" s="35"/>
       <c r="G9" s="4" t="s">
         <v>14</v>
       </c>
@@ -1092,24 +1095,24 @@
         <f t="shared" si="0"/>
         <v>0.02</v>
       </c>
-      <c r="M9" s="18">
+      <c r="M9" s="14">
         <v>2084</v>
       </c>
-      <c r="N9" s="18"/>
-      <c r="O9" s="18">
+      <c r="N9" s="14"/>
+      <c r="O9" s="14">
         <f>M9/1000</f>
         <v>2.0840000000000001</v>
       </c>
-      <c r="P9" s="18"/>
-      <c r="Q9" s="18">
+      <c r="P9" s="14"/>
+      <c r="Q9" s="14">
         <f>2*O9*(K9+L9)</f>
         <v>0.16672000000000001</v>
       </c>
-      <c r="R9" s="19"/>
-    </row>
-    <row r="10" spans="5:19" ht="18" x14ac:dyDescent="0.35">
-      <c r="E10" s="16"/>
-      <c r="F10" s="13"/>
+      <c r="R9" s="15"/>
+    </row>
+    <row r="10" spans="5:20" ht="18" x14ac:dyDescent="0.35">
+      <c r="E10" s="39"/>
+      <c r="F10" s="35"/>
       <c r="G10" s="4" t="s">
         <v>14</v>
       </c>
@@ -1130,24 +1133,24 @@
         <f t="shared" si="0"/>
         <v>0.02</v>
       </c>
-      <c r="M10" s="18">
+      <c r="M10" s="14">
         <v>2937</v>
       </c>
-      <c r="N10" s="18"/>
-      <c r="O10" s="18">
+      <c r="N10" s="14"/>
+      <c r="O10" s="14">
         <f>M10/1000</f>
         <v>2.9369999999999998</v>
       </c>
-      <c r="P10" s="18"/>
-      <c r="Q10" s="18">
+      <c r="P10" s="14"/>
+      <c r="Q10" s="14">
         <f>2*O10*(K10+L10)</f>
         <v>0.23496</v>
       </c>
-      <c r="R10" s="19"/>
-    </row>
-    <row r="11" spans="5:19" ht="18" x14ac:dyDescent="0.35">
-      <c r="E11" s="16"/>
-      <c r="F11" s="13"/>
+      <c r="R10" s="15"/>
+    </row>
+    <row r="11" spans="5:20" ht="18" x14ac:dyDescent="0.35">
+      <c r="E11" s="39"/>
+      <c r="F11" s="35"/>
       <c r="G11" s="4" t="s">
         <v>14</v>
       </c>
@@ -1168,24 +1171,27 @@
         <f t="shared" si="0"/>
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="M11" s="10">
+      <c r="M11" s="12">
         <v>700</v>
       </c>
-      <c r="N11" s="11"/>
-      <c r="O11" s="18">
+      <c r="N11" s="13"/>
+      <c r="O11" s="14">
         <f t="shared" ref="O11:O31" si="1">M11/1000</f>
         <v>0.7</v>
       </c>
-      <c r="P11" s="18"/>
-      <c r="Q11" s="18">
+      <c r="P11" s="14"/>
+      <c r="Q11" s="14">
         <f t="shared" ref="Q11:Q31" si="2">2*O11*(K11+L11)</f>
         <v>4.1999999999999996E-2</v>
       </c>
-      <c r="R11" s="19"/>
-    </row>
-    <row r="12" spans="5:19" ht="18" x14ac:dyDescent="0.35">
-      <c r="E12" s="16"/>
-      <c r="F12" s="13"/>
+      <c r="R11" s="15"/>
+      <c r="T11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="5:20" ht="18" x14ac:dyDescent="0.35">
+      <c r="E12" s="39"/>
+      <c r="F12" s="35"/>
       <c r="G12" s="4" t="s">
         <v>14</v>
       </c>
@@ -1206,24 +1212,24 @@
         <f t="shared" si="0"/>
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="M12" s="10">
+      <c r="M12" s="12">
         <v>723</v>
       </c>
-      <c r="N12" s="11"/>
-      <c r="O12" s="18">
+      <c r="N12" s="13"/>
+      <c r="O12" s="14">
         <f t="shared" si="1"/>
         <v>0.72299999999999998</v>
       </c>
-      <c r="P12" s="18"/>
-      <c r="Q12" s="18">
+      <c r="P12" s="14"/>
+      <c r="Q12" s="14">
         <f t="shared" si="2"/>
         <v>4.3379999999999995E-2</v>
       </c>
-      <c r="R12" s="19"/>
-    </row>
-    <row r="13" spans="5:19" ht="18" x14ac:dyDescent="0.35">
-      <c r="E13" s="16"/>
-      <c r="F13" s="13"/>
+      <c r="R12" s="15"/>
+    </row>
+    <row r="13" spans="5:20" ht="18" x14ac:dyDescent="0.35">
+      <c r="E13" s="39"/>
+      <c r="F13" s="35"/>
       <c r="G13" s="4" t="s">
         <v>14</v>
       </c>
@@ -1244,24 +1250,24 @@
         <f t="shared" si="0"/>
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="M13" s="10">
+      <c r="M13" s="12">
         <v>4122</v>
       </c>
-      <c r="N13" s="11"/>
-      <c r="O13" s="18">
+      <c r="N13" s="13"/>
+      <c r="O13" s="14">
         <f t="shared" si="1"/>
         <v>4.1219999999999999</v>
       </c>
-      <c r="P13" s="18"/>
-      <c r="Q13" s="18">
+      <c r="P13" s="14"/>
+      <c r="Q13" s="14">
         <f t="shared" si="2"/>
         <v>0.24731999999999998</v>
       </c>
-      <c r="R13" s="19"/>
-    </row>
-    <row r="14" spans="5:19" ht="18" x14ac:dyDescent="0.35">
-      <c r="E14" s="16"/>
-      <c r="F14" s="13"/>
+      <c r="R13" s="15"/>
+    </row>
+    <row r="14" spans="5:20" ht="18" x14ac:dyDescent="0.35">
+      <c r="E14" s="39"/>
+      <c r="F14" s="35"/>
       <c r="G14" s="4" t="s">
         <v>14</v>
       </c>
@@ -1282,24 +1288,24 @@
         <f t="shared" si="0"/>
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="M14" s="10">
+      <c r="M14" s="12">
         <v>643</v>
       </c>
-      <c r="N14" s="11"/>
-      <c r="O14" s="18">
+      <c r="N14" s="13"/>
+      <c r="O14" s="14">
         <f t="shared" si="1"/>
         <v>0.64300000000000002</v>
       </c>
-      <c r="P14" s="18"/>
-      <c r="Q14" s="18">
+      <c r="P14" s="14"/>
+      <c r="Q14" s="14">
         <f t="shared" si="2"/>
         <v>3.8579999999999996E-2</v>
       </c>
-      <c r="R14" s="19"/>
-    </row>
-    <row r="15" spans="5:19" ht="18" x14ac:dyDescent="0.35">
-      <c r="E15" s="16"/>
-      <c r="F15" s="13"/>
+      <c r="R14" s="15"/>
+    </row>
+    <row r="15" spans="5:20" ht="18" x14ac:dyDescent="0.35">
+      <c r="E15" s="39"/>
+      <c r="F15" s="35"/>
       <c r="G15" s="4" t="s">
         <v>14</v>
       </c>
@@ -1320,24 +1326,24 @@
         <f t="shared" si="0"/>
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="M15" s="10">
+      <c r="M15" s="12">
         <v>3101</v>
       </c>
-      <c r="N15" s="11"/>
-      <c r="O15" s="18">
+      <c r="N15" s="13"/>
+      <c r="O15" s="14">
         <f t="shared" si="1"/>
         <v>3.101</v>
       </c>
-      <c r="P15" s="18"/>
-      <c r="Q15" s="18">
+      <c r="P15" s="14"/>
+      <c r="Q15" s="14">
         <f t="shared" si="2"/>
         <v>0.18606</v>
       </c>
-      <c r="R15" s="19"/>
-    </row>
-    <row r="16" spans="5:19" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E16" s="16"/>
-      <c r="F16" s="13"/>
+      <c r="R15" s="15"/>
+    </row>
+    <row r="16" spans="5:20" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E16" s="39"/>
+      <c r="F16" s="35"/>
       <c r="G16" s="4" t="s">
         <v>14</v>
       </c>
@@ -1358,24 +1364,24 @@
         <f t="shared" si="0"/>
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="M16" s="10">
+      <c r="M16" s="12">
         <v>4266</v>
       </c>
-      <c r="N16" s="11"/>
-      <c r="O16" s="18">
+      <c r="N16" s="13"/>
+      <c r="O16" s="14">
         <f t="shared" si="1"/>
         <v>4.266</v>
       </c>
-      <c r="P16" s="18"/>
-      <c r="Q16" s="18">
+      <c r="P16" s="14"/>
+      <c r="Q16" s="14">
         <f t="shared" si="2"/>
         <v>0.25595999999999997</v>
       </c>
-      <c r="R16" s="19"/>
+      <c r="R16" s="15"/>
     </row>
     <row r="17" spans="5:18" ht="18" x14ac:dyDescent="0.35">
-      <c r="E17" s="16"/>
-      <c r="F17" s="13"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="35"/>
       <c r="G17" s="4" t="s">
         <v>16</v>
       </c>
@@ -1396,24 +1402,24 @@
         <f t="shared" si="0"/>
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="M17" s="28">
+      <c r="M17" s="16">
         <v>2540</v>
       </c>
-      <c r="N17" s="28"/>
-      <c r="O17" s="18">
+      <c r="N17" s="16"/>
+      <c r="O17" s="14">
         <f t="shared" si="1"/>
         <v>2.54</v>
       </c>
-      <c r="P17" s="18"/>
-      <c r="Q17" s="18">
+      <c r="P17" s="14"/>
+      <c r="Q17" s="14">
         <f t="shared" si="2"/>
         <v>0.32512000000000002</v>
       </c>
-      <c r="R17" s="19"/>
+      <c r="R17" s="15"/>
     </row>
     <row r="18" spans="5:18" ht="18" x14ac:dyDescent="0.35">
-      <c r="E18" s="16"/>
-      <c r="F18" s="13"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="35"/>
       <c r="G18" s="4" t="s">
         <v>16</v>
       </c>
@@ -1434,24 +1440,24 @@
         <f t="shared" si="0"/>
         <v>0.02</v>
       </c>
-      <c r="M18" s="18">
+      <c r="M18" s="14">
         <v>2284</v>
       </c>
-      <c r="N18" s="18"/>
-      <c r="O18" s="18">
+      <c r="N18" s="14"/>
+      <c r="O18" s="14">
         <f t="shared" si="1"/>
         <v>2.2839999999999998</v>
       </c>
-      <c r="P18" s="18"/>
-      <c r="Q18" s="18">
+      <c r="P18" s="14"/>
+      <c r="Q18" s="14">
         <f t="shared" si="2"/>
         <v>0.18271999999999999</v>
       </c>
-      <c r="R18" s="19"/>
+      <c r="R18" s="15"/>
     </row>
     <row r="19" spans="5:18" ht="18" x14ac:dyDescent="0.35">
-      <c r="E19" s="16"/>
-      <c r="F19" s="13"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="35"/>
       <c r="G19" s="4" t="s">
         <v>16</v>
       </c>
@@ -1472,24 +1478,24 @@
         <f t="shared" si="0"/>
         <v>0.02</v>
       </c>
-      <c r="M19" s="10">
+      <c r="M19" s="12">
         <v>2707</v>
       </c>
-      <c r="N19" s="11"/>
-      <c r="O19" s="18">
+      <c r="N19" s="13"/>
+      <c r="O19" s="14">
         <f t="shared" si="1"/>
         <v>2.7069999999999999</v>
       </c>
-      <c r="P19" s="18"/>
-      <c r="Q19" s="18">
+      <c r="P19" s="14"/>
+      <c r="Q19" s="14">
         <f t="shared" si="2"/>
         <v>0.21656</v>
       </c>
-      <c r="R19" s="19"/>
+      <c r="R19" s="15"/>
     </row>
     <row r="20" spans="5:18" ht="18" x14ac:dyDescent="0.35">
-      <c r="E20" s="16"/>
-      <c r="F20" s="13"/>
+      <c r="E20" s="39"/>
+      <c r="F20" s="35"/>
       <c r="G20" s="4" t="s">
         <v>16</v>
       </c>
@@ -1510,24 +1516,24 @@
         <f t="shared" si="0"/>
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="M20" s="10">
+      <c r="M20" s="12">
         <v>600</v>
       </c>
-      <c r="N20" s="11"/>
-      <c r="O20" s="18">
+      <c r="N20" s="13"/>
+      <c r="O20" s="14">
         <f t="shared" si="1"/>
         <v>0.6</v>
       </c>
-      <c r="P20" s="18"/>
-      <c r="Q20" s="18">
+      <c r="P20" s="14"/>
+      <c r="Q20" s="14">
         <f t="shared" si="2"/>
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="R20" s="19"/>
+      <c r="R20" s="15"/>
     </row>
     <row r="21" spans="5:18" ht="18" x14ac:dyDescent="0.35">
-      <c r="E21" s="16"/>
-      <c r="F21" s="13"/>
+      <c r="E21" s="39"/>
+      <c r="F21" s="35"/>
       <c r="G21" s="4" t="s">
         <v>16</v>
       </c>
@@ -1548,24 +1554,24 @@
         <f t="shared" si="0"/>
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="M21" s="10">
+      <c r="M21" s="12">
         <v>723</v>
       </c>
-      <c r="N21" s="11"/>
-      <c r="O21" s="18">
+      <c r="N21" s="13"/>
+      <c r="O21" s="14">
         <f t="shared" si="1"/>
         <v>0.72299999999999998</v>
       </c>
-      <c r="P21" s="18"/>
-      <c r="Q21" s="18">
+      <c r="P21" s="14"/>
+      <c r="Q21" s="14">
         <f t="shared" si="2"/>
         <v>4.3379999999999995E-2</v>
       </c>
-      <c r="R21" s="19"/>
+      <c r="R21" s="15"/>
     </row>
     <row r="22" spans="5:18" ht="18" x14ac:dyDescent="0.35">
-      <c r="E22" s="16"/>
-      <c r="F22" s="13"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="35"/>
       <c r="G22" s="4" t="s">
         <v>16</v>
       </c>
@@ -1586,24 +1592,24 @@
         <f t="shared" si="0"/>
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="M22" s="10">
+      <c r="M22" s="12">
         <v>4022</v>
       </c>
-      <c r="N22" s="11"/>
-      <c r="O22" s="18">
+      <c r="N22" s="13"/>
+      <c r="O22" s="14">
         <f t="shared" si="1"/>
         <v>4.0220000000000002</v>
       </c>
-      <c r="P22" s="18"/>
-      <c r="Q22" s="18">
+      <c r="P22" s="14"/>
+      <c r="Q22" s="14">
         <f t="shared" si="2"/>
         <v>0.24132000000000001</v>
       </c>
-      <c r="R22" s="19"/>
+      <c r="R22" s="15"/>
     </row>
     <row r="23" spans="5:18" ht="18" x14ac:dyDescent="0.35">
-      <c r="E23" s="16"/>
-      <c r="F23" s="13"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="35"/>
       <c r="G23" s="4" t="s">
         <v>16</v>
       </c>
@@ -1624,24 +1630,24 @@
         <f t="shared" si="0"/>
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="M23" s="10">
+      <c r="M23" s="12">
         <v>543</v>
       </c>
-      <c r="N23" s="11"/>
-      <c r="O23" s="18">
+      <c r="N23" s="13"/>
+      <c r="O23" s="14">
         <f t="shared" si="1"/>
         <v>0.54300000000000004</v>
       </c>
-      <c r="P23" s="18"/>
-      <c r="Q23" s="18">
+      <c r="P23" s="14"/>
+      <c r="Q23" s="14">
         <f t="shared" si="2"/>
         <v>3.2579999999999998E-2</v>
       </c>
-      <c r="R23" s="19"/>
+      <c r="R23" s="15"/>
     </row>
     <row r="24" spans="5:18" ht="18" x14ac:dyDescent="0.35">
-      <c r="E24" s="16"/>
-      <c r="F24" s="13"/>
+      <c r="E24" s="39"/>
+      <c r="F24" s="35"/>
       <c r="G24" s="4" t="s">
         <v>16</v>
       </c>
@@ -1662,24 +1668,24 @@
         <f t="shared" si="0"/>
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="M24" s="10">
+      <c r="M24" s="12">
         <v>3101</v>
       </c>
-      <c r="N24" s="11"/>
-      <c r="O24" s="18">
+      <c r="N24" s="13"/>
+      <c r="O24" s="14">
         <f t="shared" si="1"/>
         <v>3.101</v>
       </c>
-      <c r="P24" s="18"/>
-      <c r="Q24" s="18">
+      <c r="P24" s="14"/>
+      <c r="Q24" s="14">
         <f t="shared" si="2"/>
         <v>0.18606</v>
       </c>
-      <c r="R24" s="19"/>
+      <c r="R24" s="15"/>
     </row>
     <row r="25" spans="5:18" ht="18" x14ac:dyDescent="0.35">
-      <c r="E25" s="16"/>
-      <c r="F25" s="13"/>
+      <c r="E25" s="39"/>
+      <c r="F25" s="35"/>
       <c r="G25" s="4" t="s">
         <v>16</v>
       </c>
@@ -1700,24 +1706,24 @@
         <f t="shared" si="0"/>
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="M25" s="10">
+      <c r="M25" s="12">
         <v>4166</v>
       </c>
-      <c r="N25" s="11"/>
-      <c r="O25" s="18">
+      <c r="N25" s="13"/>
+      <c r="O25" s="14">
         <f t="shared" si="1"/>
         <v>4.1660000000000004</v>
       </c>
-      <c r="P25" s="18"/>
-      <c r="Q25" s="18">
+      <c r="P25" s="14"/>
+      <c r="Q25" s="14">
         <f t="shared" si="2"/>
         <v>0.24996000000000002</v>
       </c>
-      <c r="R25" s="19"/>
+      <c r="R25" s="15"/>
     </row>
     <row r="26" spans="5:18" ht="18" x14ac:dyDescent="0.35">
-      <c r="E26" s="16"/>
-      <c r="F26" s="13"/>
+      <c r="E26" s="39"/>
+      <c r="F26" s="35"/>
       <c r="G26" s="4" t="s">
         <v>19</v>
       </c>
@@ -1738,24 +1744,24 @@
         <f t="shared" si="0"/>
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="M26" s="10">
+      <c r="M26" s="12">
         <v>30</v>
       </c>
-      <c r="N26" s="11"/>
-      <c r="O26" s="18">
+      <c r="N26" s="13"/>
+      <c r="O26" s="14">
         <f t="shared" si="1"/>
         <v>0.03</v>
       </c>
-      <c r="P26" s="18"/>
-      <c r="Q26" s="18">
+      <c r="P26" s="14"/>
+      <c r="Q26" s="14">
         <f t="shared" si="2"/>
         <v>2.6999999999999997E-3</v>
       </c>
-      <c r="R26" s="19"/>
+      <c r="R26" s="15"/>
     </row>
     <row r="27" spans="5:18" ht="18" x14ac:dyDescent="0.35">
-      <c r="E27" s="16"/>
-      <c r="F27" s="13"/>
+      <c r="E27" s="39"/>
+      <c r="F27" s="35"/>
       <c r="G27" s="4" t="s">
         <v>19</v>
       </c>
@@ -1776,24 +1782,24 @@
         <f t="shared" si="0"/>
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="M27" s="10">
+      <c r="M27" s="12">
         <v>30</v>
       </c>
-      <c r="N27" s="11"/>
-      <c r="O27" s="18">
+      <c r="N27" s="13"/>
+      <c r="O27" s="14">
         <f t="shared" si="1"/>
         <v>0.03</v>
       </c>
-      <c r="P27" s="18"/>
-      <c r="Q27" s="18">
+      <c r="P27" s="14"/>
+      <c r="Q27" s="14">
         <f t="shared" si="2"/>
         <v>2.6999999999999997E-3</v>
       </c>
-      <c r="R27" s="19"/>
+      <c r="R27" s="15"/>
     </row>
     <row r="28" spans="5:18" ht="18" x14ac:dyDescent="0.35">
-      <c r="E28" s="16"/>
-      <c r="F28" s="13"/>
+      <c r="E28" s="39"/>
+      <c r="F28" s="35"/>
       <c r="G28" s="4" t="s">
         <v>19</v>
       </c>
@@ -1814,24 +1820,24 @@
         <f t="shared" si="0"/>
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="M28" s="10">
+      <c r="M28" s="12">
         <v>30</v>
       </c>
-      <c r="N28" s="11"/>
-      <c r="O28" s="18">
+      <c r="N28" s="13"/>
+      <c r="O28" s="14">
         <f t="shared" si="1"/>
         <v>0.03</v>
       </c>
-      <c r="P28" s="18"/>
-      <c r="Q28" s="18">
+      <c r="P28" s="14"/>
+      <c r="Q28" s="14">
         <f t="shared" si="2"/>
         <v>2.6999999999999997E-3</v>
       </c>
-      <c r="R28" s="19"/>
+      <c r="R28" s="15"/>
     </row>
     <row r="29" spans="5:18" ht="18" x14ac:dyDescent="0.35">
-      <c r="E29" s="16"/>
-      <c r="F29" s="13"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="35"/>
       <c r="G29" s="4" t="s">
         <v>19</v>
       </c>
@@ -1852,24 +1858,24 @@
         <f t="shared" si="0"/>
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="M29" s="10">
+      <c r="M29" s="12">
         <v>30</v>
       </c>
-      <c r="N29" s="11"/>
-      <c r="O29" s="18">
+      <c r="N29" s="13"/>
+      <c r="O29" s="14">
         <f t="shared" si="1"/>
         <v>0.03</v>
       </c>
-      <c r="P29" s="18"/>
-      <c r="Q29" s="18">
+      <c r="P29" s="14"/>
+      <c r="Q29" s="14">
         <f t="shared" si="2"/>
         <v>2.6999999999999997E-3</v>
       </c>
-      <c r="R29" s="19"/>
+      <c r="R29" s="15"/>
     </row>
     <row r="30" spans="5:18" ht="18" x14ac:dyDescent="0.35">
-      <c r="E30" s="16"/>
-      <c r="F30" s="13"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="35"/>
       <c r="G30" s="4" t="s">
         <v>20</v>
       </c>
@@ -1890,24 +1896,24 @@
         <f t="shared" si="0"/>
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="M30" s="10">
+      <c r="M30" s="12">
         <v>64</v>
       </c>
-      <c r="N30" s="11"/>
-      <c r="O30" s="18">
+      <c r="N30" s="13"/>
+      <c r="O30" s="14">
         <f t="shared" si="1"/>
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="P30" s="18"/>
-      <c r="Q30" s="18">
+      <c r="P30" s="14"/>
+      <c r="Q30" s="14">
         <f t="shared" si="2"/>
         <v>1.6383999999999999E-2</v>
       </c>
-      <c r="R30" s="19"/>
+      <c r="R30" s="15"/>
     </row>
     <row r="31" spans="5:18" ht="18" x14ac:dyDescent="0.35">
-      <c r="E31" s="16"/>
-      <c r="F31" s="13"/>
+      <c r="E31" s="39"/>
+      <c r="F31" s="35"/>
       <c r="G31" s="4" t="s">
         <v>20</v>
       </c>
@@ -1928,24 +1934,24 @@
         <f t="shared" si="0"/>
         <v>0.02</v>
       </c>
-      <c r="M31" s="10">
+      <c r="M31" s="12">
         <v>40</v>
       </c>
-      <c r="N31" s="11"/>
-      <c r="O31" s="18">
+      <c r="N31" s="13"/>
+      <c r="O31" s="14">
         <f t="shared" si="1"/>
         <v>0.04</v>
       </c>
-      <c r="P31" s="18"/>
-      <c r="Q31" s="18">
+      <c r="P31" s="14"/>
+      <c r="Q31" s="14">
         <f t="shared" si="2"/>
         <v>6.4000000000000003E-3</v>
       </c>
-      <c r="R31" s="19"/>
+      <c r="R31" s="15"/>
     </row>
     <row r="32" spans="5:18" ht="18" x14ac:dyDescent="0.35">
-      <c r="E32" s="16"/>
-      <c r="F32" s="13"/>
+      <c r="E32" s="39"/>
+      <c r="F32" s="35"/>
       <c r="G32" s="4" t="s">
         <v>20</v>
       </c>
@@ -1966,24 +1972,24 @@
         <f t="shared" si="0"/>
         <v>0.02</v>
       </c>
-      <c r="M32" s="18">
+      <c r="M32" s="14">
         <v>40</v>
       </c>
-      <c r="N32" s="18"/>
-      <c r="O32" s="18">
+      <c r="N32" s="14"/>
+      <c r="O32" s="14">
         <f t="shared" ref="O32" si="3">M32/1000</f>
         <v>0.04</v>
       </c>
-      <c r="P32" s="18"/>
-      <c r="Q32" s="18">
+      <c r="P32" s="14"/>
+      <c r="Q32" s="14">
         <f t="shared" ref="Q32:Q35" si="4">2*O32*(K32+L32)</f>
         <v>6.4000000000000003E-3</v>
       </c>
-      <c r="R32" s="19"/>
+      <c r="R32" s="15"/>
     </row>
     <row r="33" spans="5:18" ht="18" x14ac:dyDescent="0.35">
-      <c r="E33" s="16"/>
-      <c r="F33" s="13"/>
+      <c r="E33" s="39"/>
+      <c r="F33" s="35"/>
       <c r="G33" s="4" t="s">
         <v>20</v>
       </c>
@@ -2004,34 +2010,34 @@
         <f t="shared" ref="L33:L35" si="6">J33/1000</f>
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="M33" s="18">
+      <c r="M33" s="14">
         <v>64</v>
       </c>
-      <c r="N33" s="18"/>
-      <c r="O33" s="18">
+      <c r="N33" s="14"/>
+      <c r="O33" s="14">
         <f t="shared" ref="O33:O35" si="7">M33/1000</f>
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="P33" s="18"/>
-      <c r="Q33" s="18">
+      <c r="P33" s="14"/>
+      <c r="Q33" s="14">
         <f t="shared" si="4"/>
         <v>1.6383999999999999E-2</v>
       </c>
-      <c r="R33" s="19"/>
+      <c r="R33" s="15"/>
     </row>
     <row r="34" spans="5:18" ht="18" x14ac:dyDescent="0.35">
-      <c r="E34" s="38"/>
-      <c r="F34" s="39"/>
-      <c r="G34" s="40" t="s">
+      <c r="E34" s="40"/>
+      <c r="F34" s="36"/>
+      <c r="G34" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="H34" s="40" t="s">
+      <c r="H34" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="I34" s="41">
+      <c r="I34" s="11">
         <v>60</v>
       </c>
-      <c r="J34" s="41">
+      <c r="J34" s="11">
         <v>20</v>
       </c>
       <c r="K34" s="2">
@@ -2042,24 +2048,24 @@
         <f t="shared" si="6"/>
         <v>0.02</v>
       </c>
-      <c r="M34" s="10">
+      <c r="M34" s="12">
         <v>40</v>
       </c>
-      <c r="N34" s="11"/>
-      <c r="O34" s="18">
+      <c r="N34" s="13"/>
+      <c r="O34" s="14">
         <f t="shared" ref="O34" si="8">M34/1000</f>
         <v>0.04</v>
       </c>
-      <c r="P34" s="18"/>
-      <c r="Q34" s="18">
+      <c r="P34" s="14"/>
+      <c r="Q34" s="14">
         <f t="shared" ref="Q34" si="9">2*O34*(K34+L34)</f>
         <v>6.4000000000000003E-3</v>
       </c>
-      <c r="R34" s="19"/>
+      <c r="R34" s="15"/>
     </row>
     <row r="35" spans="5:18" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E35" s="17"/>
-      <c r="F35" s="14"/>
+      <c r="E35" s="41"/>
+      <c r="F35" s="37"/>
       <c r="G35" s="5" t="s">
         <v>20</v>
       </c>
@@ -2080,20 +2086,20 @@
         <f t="shared" si="6"/>
         <v>0.02</v>
       </c>
-      <c r="M35" s="21">
+      <c r="M35" s="26">
         <v>40</v>
       </c>
-      <c r="N35" s="21"/>
-      <c r="O35" s="21">
+      <c r="N35" s="26"/>
+      <c r="O35" s="26">
         <f t="shared" si="7"/>
         <v>0.04</v>
       </c>
-      <c r="P35" s="21"/>
-      <c r="Q35" s="23">
+      <c r="P35" s="26"/>
+      <c r="Q35" s="27">
         <f t="shared" si="4"/>
         <v>6.4000000000000003E-3</v>
       </c>
-      <c r="R35" s="24"/>
+      <c r="R35" s="28"/>
     </row>
     <row r="36" spans="5:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E36" s="6"/>
@@ -2104,26 +2110,107 @@
       <c r="J36" s="6"/>
       <c r="K36" s="6"/>
       <c r="L36" s="6"/>
-      <c r="M36" s="20"/>
-      <c r="N36" s="20"/>
-      <c r="O36" s="20"/>
-      <c r="P36" s="20"/>
-      <c r="Q36" s="21">
+      <c r="M36" s="30"/>
+      <c r="N36" s="30"/>
+      <c r="O36" s="30"/>
+      <c r="P36" s="30"/>
+      <c r="Q36" s="26">
         <f>SUM(Q8:R35)/0.9</f>
         <v>3.4415199999999997</v>
       </c>
-      <c r="R36" s="21"/>
+      <c r="R36" s="26"/>
     </row>
     <row r="37" spans="5:18" x14ac:dyDescent="0.3">
-      <c r="M37" s="22"/>
-      <c r="N37" s="22"/>
-      <c r="O37" s="22"/>
-      <c r="P37" s="22"/>
-      <c r="Q37" s="22"/>
-      <c r="R37" s="22"/>
+      <c r="M37" s="33"/>
+      <c r="N37" s="33"/>
+      <c r="O37" s="33"/>
+      <c r="P37" s="33"/>
+      <c r="Q37" s="33"/>
+      <c r="R37" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="105">
+    <mergeCell ref="M36:N36"/>
+    <mergeCell ref="O36:P36"/>
+    <mergeCell ref="Q36:R36"/>
+    <mergeCell ref="M37:N37"/>
+    <mergeCell ref="O37:P37"/>
+    <mergeCell ref="Q37:R37"/>
+    <mergeCell ref="O31:P31"/>
+    <mergeCell ref="Q31:R31"/>
+    <mergeCell ref="F8:F35"/>
+    <mergeCell ref="M33:N33"/>
+    <mergeCell ref="O33:P33"/>
+    <mergeCell ref="Q33:R33"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="M32:N32"/>
+    <mergeCell ref="O32:P32"/>
+    <mergeCell ref="Q32:R32"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="O30:P30"/>
+    <mergeCell ref="Q30:R30"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="M28:N28"/>
+    <mergeCell ref="E2:R4"/>
+    <mergeCell ref="E5:R5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="E8:E35"/>
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="M31:N31"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="Q26:R26"/>
+    <mergeCell ref="Q27:R27"/>
+    <mergeCell ref="Q28:R28"/>
+    <mergeCell ref="Q29:R29"/>
+    <mergeCell ref="Q8:R8"/>
+    <mergeCell ref="Q6:R7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="M35:N35"/>
+    <mergeCell ref="O35:P35"/>
+    <mergeCell ref="Q35:R35"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="O28:P28"/>
+    <mergeCell ref="O26:P26"/>
+    <mergeCell ref="O27:P27"/>
+    <mergeCell ref="O29:P29"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="Q11:R11"/>
+    <mergeCell ref="Q12:R12"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="Q14:R14"/>
+    <mergeCell ref="Q22:R22"/>
+    <mergeCell ref="Q23:R23"/>
+    <mergeCell ref="Q24:R24"/>
+    <mergeCell ref="Q25:R25"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="O22:P22"/>
     <mergeCell ref="M34:N34"/>
     <mergeCell ref="O34:P34"/>
     <mergeCell ref="Q34:R34"/>
@@ -2148,87 +2235,6 @@
     <mergeCell ref="Q19:R19"/>
     <mergeCell ref="Q20:R20"/>
     <mergeCell ref="Q21:R21"/>
-    <mergeCell ref="Q22:R22"/>
-    <mergeCell ref="Q23:R23"/>
-    <mergeCell ref="Q24:R24"/>
-    <mergeCell ref="Q25:R25"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="Q8:R8"/>
-    <mergeCell ref="Q6:R7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="M35:N35"/>
-    <mergeCell ref="O35:P35"/>
-    <mergeCell ref="Q35:R35"/>
-    <mergeCell ref="E2:R4"/>
-    <mergeCell ref="E5:R5"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="Q9:R9"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="M36:N36"/>
-    <mergeCell ref="O36:P36"/>
-    <mergeCell ref="Q36:R36"/>
-    <mergeCell ref="M37:N37"/>
-    <mergeCell ref="O37:P37"/>
-    <mergeCell ref="Q37:R37"/>
-    <mergeCell ref="O31:P31"/>
-    <mergeCell ref="Q31:R31"/>
-    <mergeCell ref="F8:F35"/>
-    <mergeCell ref="E8:E35"/>
-    <mergeCell ref="M33:N33"/>
-    <mergeCell ref="O33:P33"/>
-    <mergeCell ref="Q33:R33"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="M32:N32"/>
-    <mergeCell ref="O32:P32"/>
-    <mergeCell ref="Q32:R32"/>
-    <mergeCell ref="M30:N30"/>
-    <mergeCell ref="O30:P30"/>
-    <mergeCell ref="Q30:R30"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="M28:N28"/>
-    <mergeCell ref="M29:N29"/>
-    <mergeCell ref="M31:N31"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="Q26:R26"/>
-    <mergeCell ref="Q27:R27"/>
-    <mergeCell ref="Q28:R28"/>
-    <mergeCell ref="Q29:R29"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="O28:P28"/>
-    <mergeCell ref="O26:P26"/>
-    <mergeCell ref="O27:P27"/>
-    <mergeCell ref="O29:P29"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="O16:P16"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="Q11:R11"/>
-    <mergeCell ref="Q12:R12"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="Q14:R14"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="E36:R37 I7:P7 E2:R5 G9:R10 E8:R8 E6:Q6 G32:R33 O11:R31 G11:M16 G19:M31 G17:N18 G35:R35 G34:M34 O34:R34">

</xml_diff>